<commit_message>
feat(programareProcedurala/practica): added the final report and updated excel
</commit_message>
<xml_diff>
--- a/programareProcedurala/practica/bauturi.xlsx
+++ b/programareProcedurala/practica/bauturi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L19_PC09\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCE8C79-430E-4584-86C3-59DA682857C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21678E5D-E9EE-42B9-90CA-46B6FB9B0465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5DA94CAC-810B-40DD-AD00-7969FF0F1961}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DA94CAC-810B-40DD-AD00-7969FF0F1961}"/>
   </bookViews>
   <sheets>
     <sheet name="Baut" sheetId="1" r:id="rId1"/>
@@ -51,6 +51,30 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>L19_PC09</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{F4C2BFC2-B62A-4731-A5AD-C4CE3CF3DBAA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
@@ -203,7 +227,7 @@
     <numFmt numFmtId="164" formatCode="[$MDL]\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$€-2]\ #,##0.00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +242,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1194,7 +1224,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$B$22" fmlaRange="Baut!$I$3:$I$17" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="22" fmlaLink="$B$22" fmlaRange="Baut!$I$3:$I$17" noThreeD="1" sel="8" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1238,15 +1268,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$B$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$B$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$B$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3141,7 +3171,7 @@
               <a:picLocks noChangeAspect="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Pictures" spid="_x0000_s3097"/>
+                  <a14:cameraTool cellRange="Pictures" spid="_x0000_s3101"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -3555,12 +3585,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D0CE3C-C051-4567-8ABA-A3C31C3074C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D0CE3C-C051-4567-8ABA-A3C31C3074C9}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3961,11 +3991,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="4">
-    <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4252,8 +4283,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4299,11 +4330,11 @@
       </c>
       <c r="E2" cm="1">
         <f t="array" ref="E2">IF(COUNTIF(Table4[Status], TRUE)=0, 0, SUM(SUMIFS(Livr[Cantitate Livrata], Livr[id_baut], _xlfn._xlws.FILTER(_xlfn.XLOOKUP(Table4[Denumire], Baut[Denumire], Baut[id_baut], ""), Table4[Status]))))</f>
-        <v>0</v>
+        <v>26.55</v>
       </c>
       <c r="F2" s="1" cm="1">
         <f t="array" ref="F2">IF(COUNTIF(Table4[Status], TRUE)=0, 0, SUM(SUMIFS(Livr[Suma], Livr[id_baut], _xlfn._xlws.FILTER(_xlfn.XLOOKUP(Table4[Denumire], Baut[Denumire], Baut[id_baut]), Table4[Status])))) * 19.55</f>
-        <v>0</v>
+        <v>55.145000000000003</v>
       </c>
       <c r="H2" t="str" cm="1">
         <f t="array" ref="H2">INDEX(Baut[Denumire],ROW()-ROW(Table5[[#Headers],[Denumire]]))</f>
@@ -4350,7 +4381,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="str" cm="1">
         <f t="array" ref="C5">INDEX(Baut[Denumire],ROW()-ROW(Table4[[#Headers],[Denumire]]))</f>
@@ -4367,7 +4398,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="str" cm="1">
         <f t="array" ref="C6">INDEX(Baut[Denumire],ROW()-ROW(Table4[[#Headers],[Denumire]]))</f>
@@ -4384,7 +4415,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" ref="C7">INDEX(Baut[Denumire],ROW()-ROW(Table4[[#Headers],[Denumire]]))</f>
@@ -4562,11 +4593,11 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C22" t="str" cm="1">
         <f t="array" ref="C22">INDEX(Table7[Denumire],B22)</f>
-        <v>CocaCola</v>
+        <v>GuraCainarului</v>
       </c>
     </row>
   </sheetData>
@@ -4710,7 +4741,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3083" r:id="rId9" name="Check Box 2">
+            <control shapeId="3083" r:id="rId9" name="Check Box 11">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4732,7 +4763,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3084" r:id="rId10" name="Check Box 2">
+            <control shapeId="3084" r:id="rId10" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4754,7 +4785,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3085" r:id="rId11" name="Check Box 2">
+            <control shapeId="3085" r:id="rId11" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4776,7 +4807,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3086" r:id="rId12" name="Check Box 2">
+            <control shapeId="3086" r:id="rId12" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4798,7 +4829,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3087" r:id="rId13" name="Check Box 2">
+            <control shapeId="3087" r:id="rId13" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4820,7 +4851,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3088" r:id="rId14" name="Check Box 2">
+            <control shapeId="3088" r:id="rId14" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4842,7 +4873,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3089" r:id="rId15" name="Check Box 2">
+            <control shapeId="3089" r:id="rId15" name="Check Box 17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4864,7 +4895,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3090" r:id="rId16" name="Check Box 2">
+            <control shapeId="3090" r:id="rId16" name="Check Box 18">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4886,7 +4917,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3091" r:id="rId17" name="Check Box 2">
+            <control shapeId="3091" r:id="rId17" name="Check Box 19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4908,7 +4939,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="3092" r:id="rId18" name="Check Box 2">
+            <control shapeId="3092" r:id="rId18" name="Check Box 20">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>